<commit_message>
feat: adicionado funcionalidade de gerar planilha, refatoração de código em classes e ativando scroll do mouse para linux
</commit_message>
<xml_diff>
--- a/data/output/PRODUTIVIDADE.xlsx
+++ b/data/output/PRODUTIVIDADE.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>21 de agosto atÃ© 27</t>
+          <t>21 de agosto até 27</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -553,7 +553,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Em cursos na verdade nÃ£o foi nenhum curso, foi debian, obsidian, itp, C e git</t>
+          <t>Em cursos na verdade não foi nenhum curso, foi debian, obsidian, itp, C e git</t>
         </is>
       </c>
       <c r="M2" t="n">
@@ -582,7 +582,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>28 atÃ© 3 de setembro</t>
+          <t>28 até 3 de setembro</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -614,7 +614,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Cursos foi a Proz, e foquei mais em CÃ¡lculo pois teoricamente teriamos prova de cÃ¡lculo na prÃ³xima semana</t>
+          <t>Cursos foi a Proz, e foquei mais em Cálculo pois teoricamente teriamos prova de cálculo na próxima semana</t>
         </is>
       </c>
       <c r="M3" t="n">
@@ -643,7 +643,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4 atÃ© 10 de setembro</t>
+          <t>4 até 10 de setembro</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -675,7 +675,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Estudei muito fmc pois tinha lista dela para entregar segunda, e cÃ¡lculo pois seria prova de Samyr na prÃ³xima semana</t>
+          <t>Estudei muito fmc pois tinha lista dela para entregar segunda, e cálculo pois seria prova de Samyr na próxima semana</t>
         </is>
       </c>
       <c r="M4" t="n">
@@ -704,7 +704,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>10 atÃ© 17 de setembro</t>
+          <t>10 até 17 de setembro</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -736,7 +736,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Tive duas provas na semana (FMC e CÃ¡lculo), portanto apÃ³s elas planejava descansar, teve aniversÃ¡rio de pai fui para Genipabu no FDS e ainda teve as palestras da IEEE na quinta</t>
+          <t>Tive duas provas na semana (FMC e Cálculo), portanto após elas planejava descansar, teve aniversário de pai fui para Genipabu no FDS e ainda teve as palestras da IEEE na quinta</t>
         </is>
       </c>
       <c r="M5" t="n">
@@ -765,7 +765,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>17 atÃ© 24 de setembro</t>
+          <t>17 até 24 de setembro</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -797,7 +797,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>As questÃµes de itp tavam muito difÃ­cil, prÃ© prova do detran, itp, fmc e cansaÃ§o</t>
+          <t>As questões de itp tavam muito difícil, pré prova do detran, itp, fmc e cansaço</t>
         </is>
       </c>
       <c r="M6" t="n">
@@ -826,7 +826,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>24 atÃ© 1 de outubro</t>
+          <t>24 até 1 de outubro</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -887,7 +887,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1 atÃ© 8 de outubro</t>
+          <t>1 até 8 de outubro</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -919,7 +919,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Tive duas provas (FMC e CÃ¡lculo) e tive as questÃµes mais difÃ­ceis da vida em itp(criptografia) tia no domingo</t>
+          <t>Tive duas provas (FMC e Cálculo) e tive as questões mais difíceis da vida em itp(criptografia) tia no domingo</t>
         </is>
       </c>
       <c r="M8" t="n">
@@ -948,7 +948,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>8 atÃ© 15 de outubro</t>
+          <t>8 até 15 de outubro</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -980,7 +980,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Fiquei doente com distÃºrbio do sono(sexta) EspÃ­rito quebrado cansaÃ§o eclipse sÃ¡bado</t>
+          <t>Fiquei doente com distúrbio do sono(sexta) Espírito quebrado cansaço eclipse sábado</t>
         </is>
       </c>
       <c r="M9" t="n">
@@ -1009,7 +1009,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>15 atÃ© 22 de outubro</t>
+          <t>15 até 22 de outubro</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -1041,7 +1041,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Teve todo o negÃ³cio da proz de fazer o css da menina lÃ¡ e o html tbm, e reuniÃ£o da petcc na quarta alÃ©m de eu tÃ¡ dirigindo sÃ¡bado e domingo</t>
+          <t>Teve todo o negócio da proz de fazer o css da menina lá e o html tbm, e reunião da petcc na quarta além de eu tá dirigindo sábado e domingo</t>
         </is>
       </c>
       <c r="M10" t="n">
@@ -1070,7 +1070,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>22 atÃ© 29 de outubro</t>
+          <t>22 até 29 de outubro</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -1102,7 +1102,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Tive muitos problemas com as listas de itp acumuladas(struct e ponteiros) alÃ©m de ter prova de FMC na prÃ³xima semana + exaustÃ£o mental, ademais adicionei a label leituras antes estava contabilizando ela em currÃ­culo</t>
+          <t>Tive muitos problemas com as listas de itp acumuladas(struct e ponteiros) além de ter prova de FMC na próxima semana + exaustão mental, ademais adicionei a label leituras antes estava contabilizando ela em currículo</t>
         </is>
       </c>
       <c r="M11" t="n">
@@ -1131,7 +1131,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>29 atÃ© 5 de novembro</t>
+          <t>29 até 5 de novembro</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5 atÃ© 12 de novembro</t>
+          <t>5 até 12 de novembro</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -1224,7 +1224,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Pensava que ia ter prova de itp na semana mas o professor adiou, ainda teve prova de cÃ¡lculo na sexta e sÃ¡bado e domingo nÃ£o consegui estudar pq teria prova prÃ¡tica do detran na segundo, assim a parte de leitura Ã© sÃ³ PLE</t>
+          <t>Pensava que ia ter prova de itp na semana mas o professor adiou, ainda teve prova de cálculo na sexta e sábado e domingo não consegui estudar pq teria prova prática do detran na segundo, assim a parte de leitura é só PLE</t>
         </is>
       </c>
       <c r="M13" t="n">
@@ -1253,7 +1253,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>12 atÃ© 19 de novembro</t>
+          <t>12 até 19 de novembro</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Tive a prova do detran na segunda o que me deixou muito ansioso, fui pra igreja tambÃ©m teve uns aniversÃ¡rios e saiu o resultado do detran tambÃ©m o que me fez desopilar</t>
+          <t>Tive a prova do detran na segunda o que me deixou muito ansioso, fui pra igreja também teve uns aniversários e saiu o resultado do detran também o que me fez desopilar</t>
         </is>
       </c>
       <c r="M14" t="n">
@@ -1314,7 +1314,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>19 atÃ© 26 de novembro</t>
+          <t>19 até 26 de novembro</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Fui para vÃ³ damiana na segunda feira pois pensava que ia ter prova de itp na segunda, mas na realidade foi online, foi uma semana bem complicada mentalmente, eu estava me sentindo muito mal e teve o show do titÃ£s sÃ¡bado</t>
+          <t>Fui para vó damiana na segunda feira pois pensava que ia ter prova de itp na segunda, mas na realidade foi online, foi uma semana bem complicada mentalmente, eu estava me sentindo muito mal e teve o show do titãs sábado</t>
         </is>
       </c>
       <c r="M15" t="n">
@@ -1375,7 +1375,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>26 atÃ© 3 de dezembro</t>
+          <t>26 até 3 de dezembro</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -1407,7 +1407,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Projeto de ITP alÃ©m de muita coisa pra fazer que me sobrecarregou, meu aniversÃ¡rio foi domingo</t>
+          <t>Projeto de ITP além de muita coisa pra fazer que me sobrecarregou, meu aniversário foi domingo</t>
         </is>
       </c>
       <c r="M16" t="n">
@@ -1436,7 +1436,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>3 atÃ© 10 de dezembro</t>
+          <t>3 até 10 de dezembro</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -1468,7 +1468,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Teve os minicursos da pet na quinta e sexta que comeram muito tempo e eu considerei eles como curriculo, teve o projeto de itp e eu ia ter a prova de fmc na segunda da prÃ³xima semana</t>
+          <t>Teve os minicursos da pet na quinta e sexta que comeram muito tempo e eu considerei eles como curriculo, teve o projeto de itp e eu ia ter a prova de fmc na segunda da próxima semana</t>
         </is>
       </c>
       <c r="M17" t="n">

</xml_diff>